<commit_message>
✨ fix(barrett_calculator.py): reduce sleep duration for improved performance
</commit_message>
<xml_diff>
--- a/APACdata.xlsx
+++ b/APACdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yokam\PycharmProjects\BarrettAutomate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3053DCAE-38FD-4845-AC4D-8B4F14638D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47659BE2-A3D8-4C8C-842A-EFFD25669B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1560" windowWidth="22890" windowHeight="11670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-690" yWindow="3735" windowWidth="25215" windowHeight="11670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="36" r:id="rId1"/>
@@ -37,68 +37,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
-  <si>
-    <t>attack1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="49">
+  <si>
+    <t>Optic</t>
+  </si>
+  <si>
+    <t>Biconvex</t>
+  </si>
+  <si>
+    <t>PatientName</t>
+  </si>
+  <si>
+    <t>AConstant</t>
+  </si>
+  <si>
+    <t>IOLPower</t>
+  </si>
+  <si>
+    <t>AxialLength_R</t>
+  </si>
+  <si>
+    <t>MeasuredK1_R</t>
+  </si>
+  <si>
+    <t>MeasuredK2_R</t>
+  </si>
+  <si>
+    <t>OpticalACD_R</t>
+  </si>
+  <si>
+    <t>Refraction_R</t>
+  </si>
+  <si>
+    <t>DoctorName</t>
+  </si>
+  <si>
+    <t>PatientID</t>
+  </si>
+  <si>
+    <t>LensFactor</t>
+  </si>
+  <si>
+    <t>Refraction</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>attack2</t>
-  </si>
-  <si>
-    <t>Optic</t>
-  </si>
-  <si>
-    <t>Biconvex</t>
-  </si>
-  <si>
-    <t>PatientName</t>
-  </si>
-  <si>
-    <t>AConstant</t>
-  </si>
-  <si>
-    <t>IOLPower</t>
-  </si>
-  <si>
-    <t>Refraction</t>
-  </si>
-  <si>
-    <t>AxialLength_R</t>
-  </si>
-  <si>
-    <t>MeasuredK1_R</t>
-  </si>
-  <si>
-    <t>MeasuredK2_R</t>
-  </si>
-  <si>
-    <t>OpticalACD_R</t>
-  </si>
-  <si>
-    <t>Refraction_R</t>
-  </si>
-  <si>
-    <t>DoctorName</t>
-  </si>
-  <si>
-    <t>PatientID</t>
-  </si>
-  <si>
-    <t>LensFactor</t>
-  </si>
-  <si>
-    <t>LAKADA</t>
+    <t>follow01</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LFKFDF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>follow02</t>
+  </si>
+  <si>
+    <t>follow03</t>
+  </si>
+  <si>
+    <t>follow04</t>
+  </si>
+  <si>
+    <t>follow05</t>
+  </si>
+  <si>
+    <t>follow06</t>
+  </si>
+  <si>
+    <t>follow07</t>
+  </si>
+  <si>
+    <t>follow08</t>
+  </si>
+  <si>
+    <t>follow09</t>
+  </si>
+  <si>
+    <t>follow10</t>
+  </si>
+  <si>
+    <t>follow11</t>
+  </si>
+  <si>
+    <t>follow12</t>
+  </si>
+  <si>
+    <t>follow13</t>
+  </si>
+  <si>
+    <t>follow14</t>
+  </si>
+  <si>
+    <t>follow15</t>
+  </si>
+  <si>
+    <t>follow16</t>
+  </si>
+  <si>
+    <t>follow17</t>
+  </si>
+  <si>
+    <t>follow18</t>
+  </si>
+  <si>
+    <t>follow19</t>
+  </si>
+  <si>
+    <t>follow20</t>
+  </si>
+  <si>
+    <t>follow21</t>
+  </si>
+  <si>
+    <t>follow22</t>
+  </si>
+  <si>
+    <t>follow23</t>
+  </si>
+  <si>
+    <t>follow24</t>
+  </si>
+  <si>
+    <t>follow25</t>
+  </si>
+  <si>
+    <t>follow26</t>
+  </si>
+  <si>
+    <t>follow27</t>
+  </si>
+  <si>
+    <t>follow28</t>
+  </si>
+  <si>
+    <t>follow29</t>
+  </si>
+  <si>
+    <t>follow30</t>
+  </si>
+  <si>
+    <t>follow31</t>
+  </si>
+  <si>
+    <t>follow32</t>
+  </si>
+  <si>
+    <t>follow33</t>
+  </si>
+  <si>
+    <t>follow34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="178" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -172,7 +270,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -204,13 +302,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="標準 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -521,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -541,57 +652,57 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1">
         <v>105737</v>
       </c>
-      <c r="D2" s="1">
-        <v>1.83</v>
+      <c r="D2" s="11">
+        <v>1.885</v>
       </c>
       <c r="E2" s="9">
         <v>119</v>
@@ -600,67 +711,1280 @@
         <v>23.04</v>
       </c>
       <c r="G2" s="7">
-        <v>44.75</v>
+        <v>45.25</v>
       </c>
       <c r="H2" s="7">
-        <v>44.25</v>
+        <v>43.25</v>
       </c>
       <c r="I2" s="7">
-        <v>2.1800000000000002</v>
+        <v>2.33</v>
       </c>
       <c r="J2" s="7">
-        <v>-0.03</v>
+        <v>-0.5</v>
       </c>
       <c r="K2" s="9">
-        <v>21.5</v>
+        <v>22.5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
-        <v>133873</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.83</v>
+        <v>132594</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1.885</v>
       </c>
       <c r="E3" s="9">
         <v>119</v>
       </c>
       <c r="F3" s="7">
-        <v>23.17</v>
+        <v>21.68</v>
       </c>
       <c r="G3" s="7">
-        <v>43.75</v>
+        <v>46.5</v>
       </c>
       <c r="H3" s="7">
-        <v>44.5</v>
+        <v>48.25</v>
       </c>
       <c r="I3" s="7">
-        <v>1.81</v>
+        <v>3.05</v>
       </c>
       <c r="J3" s="7">
-        <v>-0.53</v>
+        <v>-0.43</v>
       </c>
       <c r="K3" s="9">
+        <v>24</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>133873</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E4" s="9">
+        <v>119</v>
+      </c>
+      <c r="F4" s="7">
+        <v>22.79</v>
+      </c>
+      <c r="G4" s="7">
+        <v>44.25</v>
+      </c>
+      <c r="H4" s="7">
+        <v>44</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2.44</v>
+      </c>
+      <c r="J4" s="6">
+        <v>-0.11</v>
+      </c>
+      <c r="K4" s="9">
+        <v>23</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>133854</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E5" s="9">
+        <v>119</v>
+      </c>
+      <c r="F5" s="7">
+        <v>21.05</v>
+      </c>
+      <c r="G5" s="7">
+        <v>46.75</v>
+      </c>
+      <c r="H5" s="7">
+        <v>47.75</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="J5" s="6">
+        <v>-0.87</v>
+      </c>
+      <c r="K5" s="9">
+        <v>27</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>35135</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E6" s="9">
+        <v>119</v>
+      </c>
+      <c r="F6" s="7">
+        <v>21.78</v>
+      </c>
+      <c r="G6" s="7">
+        <v>43.1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>45</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2.75</v>
+      </c>
+      <c r="J6" s="6">
+        <v>-0.24</v>
+      </c>
+      <c r="K6" s="9">
+        <v>28</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2">
+        <v>23574</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1.62</v>
+      </c>
+      <c r="E7" s="9">
+        <v>118.5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>23.04</v>
+      </c>
+      <c r="G7" s="7">
+        <v>42.72</v>
+      </c>
+      <c r="H7" s="7">
+        <v>43.55</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2.29</v>
+      </c>
+      <c r="J7" s="6">
+        <v>-0.48</v>
+      </c>
+      <c r="K7" s="9">
+        <v>23</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2">
+        <v>143993</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E8" s="9">
+        <v>119</v>
+      </c>
+      <c r="F8" s="7">
+        <v>24.09</v>
+      </c>
+      <c r="G8" s="7">
+        <v>43.44</v>
+      </c>
+      <c r="H8" s="7">
+        <v>43.83</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2.29</v>
+      </c>
+      <c r="J8" s="6">
+        <v>-1.3</v>
+      </c>
+      <c r="K8" s="9">
+        <v>21</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>3</v>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>47248</v>
+      </c>
+      <c r="D9" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E9" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F9" s="7">
+        <v>22.17</v>
+      </c>
+      <c r="G9" s="7">
+        <v>43.83</v>
+      </c>
+      <c r="H9" s="7">
+        <v>44.53</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J9" s="6">
+        <v>-0.6</v>
+      </c>
+      <c r="K9" s="9">
+        <v>26</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2">
+        <v>110627</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E10" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F10" s="7">
+        <v>21.69</v>
+      </c>
+      <c r="G10" s="7">
+        <v>44.29</v>
+      </c>
+      <c r="H10" s="7">
+        <v>48.49</v>
+      </c>
+      <c r="I10" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="J10" s="6">
+        <v>-1.04</v>
+      </c>
+      <c r="K10" s="9">
+        <v>26</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>161460</v>
+      </c>
+      <c r="D11" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E11" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F11" s="7">
+        <v>23.65</v>
+      </c>
+      <c r="G11" s="7">
+        <v>42.35</v>
+      </c>
+      <c r="H11" s="7">
+        <v>42.72</v>
+      </c>
+      <c r="I11" s="7">
+        <v>2.13</v>
+      </c>
+      <c r="J11" s="6">
+        <v>-1.24</v>
+      </c>
+      <c r="K11" s="9">
+        <v>23.5</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2">
+        <v>161554</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E12" s="9">
+        <v>119</v>
+      </c>
+      <c r="F12" s="7">
+        <v>21.55</v>
+      </c>
+      <c r="G12" s="7">
+        <v>44.47</v>
+      </c>
+      <c r="H12" s="7">
+        <v>46.75</v>
+      </c>
+      <c r="I12" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J12" s="6">
+        <v>-0.94</v>
+      </c>
+      <c r="K12" s="9">
+        <v>27</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2">
+        <v>166237</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E13" s="9">
+        <v>119</v>
+      </c>
+      <c r="F13" s="7">
+        <v>22.41</v>
+      </c>
+      <c r="G13" s="7">
+        <v>45.18</v>
+      </c>
+      <c r="H13" s="7">
+        <v>45.55</v>
+      </c>
+      <c r="I13" s="7">
+        <v>2.63</v>
+      </c>
+      <c r="J13" s="6">
+        <v>-0.11</v>
+      </c>
+      <c r="K13" s="9">
+        <v>23</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2">
+        <v>166886</v>
+      </c>
+      <c r="D14" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E14" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F14" s="7">
+        <v>22.79</v>
+      </c>
+      <c r="G14" s="7">
+        <v>42.99</v>
+      </c>
+      <c r="H14" s="7">
+        <v>43.38</v>
+      </c>
+      <c r="I14" s="7">
+        <v>2.14</v>
+      </c>
+      <c r="J14" s="6">
+        <v>-0.44</v>
+      </c>
+      <c r="K14" s="9">
+        <v>24.5</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2">
+        <v>167592</v>
+      </c>
+      <c r="D15" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E15" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F15" s="7">
+        <v>22.61</v>
+      </c>
+      <c r="G15" s="7">
+        <v>43.49</v>
+      </c>
+      <c r="H15" s="7">
+        <v>44.58</v>
+      </c>
+      <c r="I15" s="7">
+        <v>2.48</v>
+      </c>
+      <c r="J15" s="6">
+        <v>-0.88</v>
+      </c>
+      <c r="K15" s="9">
+        <v>25</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>51973</v>
+      </c>
+      <c r="D16" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E16" s="9">
+        <v>119</v>
+      </c>
+      <c r="F16" s="7">
+        <v>21.25</v>
+      </c>
+      <c r="G16" s="7">
+        <v>45.61</v>
+      </c>
+      <c r="H16" s="7">
+        <v>47.2</v>
+      </c>
+      <c r="I16" s="7">
+        <v>2.29</v>
+      </c>
+      <c r="J16" s="6">
+        <v>-0.64</v>
+      </c>
+      <c r="K16" s="9">
+        <v>27</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2">
+        <v>145550</v>
+      </c>
+      <c r="D17" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E17" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F17" s="7">
+        <v>22.04</v>
+      </c>
+      <c r="G17" s="7">
+        <v>44.12</v>
+      </c>
+      <c r="H17" s="7">
+        <v>45.36</v>
+      </c>
+      <c r="I17" s="7">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="J17" s="6">
+        <v>-0.61</v>
+      </c>
+      <c r="K17" s="9">
+        <v>26</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2">
+        <v>173959</v>
+      </c>
+      <c r="D18" s="11">
+        <v>2.145</v>
+      </c>
+      <c r="E18" s="9">
+        <v>119.5</v>
+      </c>
+      <c r="F18" s="7">
+        <v>22.75</v>
+      </c>
+      <c r="G18" s="7">
+        <v>43.38</v>
+      </c>
+      <c r="H18" s="7">
+        <v>43.95</v>
+      </c>
+      <c r="I18" s="7">
+        <v>2.36</v>
+      </c>
+      <c r="J18" s="6">
+        <v>-1.01</v>
+      </c>
+      <c r="K18" s="9">
+        <v>25</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2">
+        <v>174163</v>
+      </c>
+      <c r="D19" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E19" s="9">
+        <v>119</v>
+      </c>
+      <c r="F19" s="7">
+        <v>22.47</v>
+      </c>
+      <c r="G19" s="7">
+        <v>43.32</v>
+      </c>
+      <c r="H19" s="7">
+        <v>44.53</v>
+      </c>
+      <c r="I19" s="7">
+        <v>2.34</v>
+      </c>
+      <c r="J19" s="6">
+        <v>-0.98</v>
+      </c>
+      <c r="K19" s="9">
+        <v>25.5</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2">
+        <v>28886</v>
+      </c>
+      <c r="D20" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E20" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F20" s="7">
+        <v>21.53</v>
+      </c>
+      <c r="G20" s="7">
+        <v>46.23</v>
+      </c>
+      <c r="H20" s="7">
+        <v>47.87</v>
+      </c>
+      <c r="I20" s="7">
+        <v>2.16</v>
+      </c>
+      <c r="J20" s="6">
+        <v>-0.81</v>
+      </c>
+      <c r="K20" s="9">
+        <v>25.5</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2">
+        <v>177432</v>
+      </c>
+      <c r="D21" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E21" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F21" s="7">
+        <v>22.97</v>
+      </c>
+      <c r="G21" s="7">
+        <v>43.77</v>
+      </c>
+      <c r="H21" s="7">
+        <v>45.92</v>
+      </c>
+      <c r="I21" s="7">
+        <v>2.39</v>
+      </c>
+      <c r="J21" s="6">
+        <v>-0.63</v>
+      </c>
+      <c r="K21" s="9">
+        <v>22.5</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="2">
+        <v>178621</v>
+      </c>
+      <c r="D22" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E22" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F22" s="7">
+        <v>21.95</v>
+      </c>
+      <c r="G22" s="7">
+        <v>45.67</v>
+      </c>
+      <c r="H22" s="7">
+        <v>46.87</v>
+      </c>
+      <c r="I22" s="7">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="J22" s="6">
+        <v>-0.64</v>
+      </c>
+      <c r="K22" s="9">
+        <v>24.5</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="2">
+        <v>178965</v>
+      </c>
+      <c r="D23" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E23" s="9">
+        <v>119</v>
+      </c>
+      <c r="F23" s="7">
+        <v>22.03</v>
+      </c>
+      <c r="G23" s="7">
+        <v>43.21</v>
+      </c>
+      <c r="H23" s="7">
+        <v>44.18</v>
+      </c>
+      <c r="I23" s="7">
+        <v>2.13</v>
+      </c>
+      <c r="J23" s="6">
+        <v>-0.2</v>
+      </c>
+      <c r="K23" s="9">
+        <v>26.5</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2">
+        <v>184985</v>
+      </c>
+      <c r="D24" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E24" s="9">
+        <v>119</v>
+      </c>
+      <c r="F24" s="7">
+        <v>21.58</v>
+      </c>
+      <c r="G24" s="7">
+        <v>44.53</v>
+      </c>
+      <c r="H24" s="7">
+        <v>46.11</v>
+      </c>
+      <c r="I24" s="7">
+        <v>2.36</v>
+      </c>
+      <c r="J24" s="6">
+        <v>-0.73</v>
+      </c>
+      <c r="K24" s="9">
+        <v>27</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2">
+        <v>186160</v>
+      </c>
+      <c r="D25" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E25" s="9">
+        <v>119</v>
+      </c>
+      <c r="F25" s="7">
+        <v>22.36</v>
+      </c>
+      <c r="G25" s="7">
+        <v>44.76</v>
+      </c>
+      <c r="H25" s="7">
+        <v>45.3</v>
+      </c>
+      <c r="I25" s="7">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="J25" s="6">
+        <v>-0.11</v>
+      </c>
+      <c r="K25" s="9">
+        <v>23.5</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2">
+        <v>96698</v>
+      </c>
+      <c r="D26" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E26" s="9">
+        <v>119</v>
+      </c>
+      <c r="F26" s="7">
+        <v>23.37</v>
+      </c>
+      <c r="G26" s="7">
+        <v>42.67</v>
+      </c>
+      <c r="H26" s="7">
+        <v>43.27</v>
+      </c>
+      <c r="I26" s="7">
+        <v>2.54</v>
+      </c>
+      <c r="J26" s="6">
+        <v>-0.16</v>
+      </c>
+      <c r="K26" s="9">
+        <v>22.5</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="2">
+        <v>125842</v>
+      </c>
+      <c r="D27" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E27" s="9">
+        <v>119</v>
+      </c>
+      <c r="F27" s="7">
+        <v>22.3</v>
+      </c>
+      <c r="G27" s="7">
+        <v>45.18</v>
+      </c>
+      <c r="H27" s="7">
+        <v>45.42</v>
+      </c>
+      <c r="I27" s="7">
+        <v>2.52</v>
+      </c>
+      <c r="J27" s="6">
+        <v>-0.08</v>
+      </c>
+      <c r="K27" s="9">
+        <v>23.5</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="2">
+        <v>192766</v>
+      </c>
+      <c r="D28" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E28" s="9">
+        <v>119</v>
+      </c>
+      <c r="F28" s="7">
+        <v>22.11</v>
+      </c>
+      <c r="G28" s="7">
+        <v>45.55</v>
+      </c>
+      <c r="H28" s="7">
+        <v>46.17</v>
+      </c>
+      <c r="I28" s="7">
+        <v>2.38</v>
+      </c>
+      <c r="J28" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="K28" s="9">
+        <v>23.5</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="2">
+        <v>193016</v>
+      </c>
+      <c r="D29" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E29" s="9">
+        <v>119</v>
+      </c>
+      <c r="F29" s="7">
+        <v>22.12</v>
+      </c>
+      <c r="G29" s="7">
+        <v>45.06</v>
+      </c>
+      <c r="H29" s="7">
+        <v>45.79</v>
+      </c>
+      <c r="I29" s="7">
+        <v>2.29</v>
+      </c>
+      <c r="J29" s="6">
+        <v>-0.05</v>
+      </c>
+      <c r="K29" s="9">
+        <v>24</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="2">
+        <v>10137</v>
+      </c>
+      <c r="D30" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E30" s="9">
+        <v>119</v>
+      </c>
+      <c r="F30" s="7">
+        <v>22.78</v>
+      </c>
+      <c r="G30" s="7">
+        <v>43.77</v>
+      </c>
+      <c r="H30" s="7">
+        <v>44.94</v>
+      </c>
+      <c r="I30" s="7">
+        <v>2.54</v>
+      </c>
+      <c r="J30" s="6">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="K30" s="9">
+        <v>23</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="2">
+        <v>198772</v>
+      </c>
+      <c r="D31" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E31" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F31" s="7">
+        <v>21.49</v>
+      </c>
+      <c r="G31" s="7">
+        <v>42.08</v>
+      </c>
+      <c r="H31" s="7">
+        <v>42.94</v>
+      </c>
+      <c r="I31" s="7">
+        <v>2.19</v>
+      </c>
+      <c r="J31" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="K31" s="9">
+        <v>30</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="2">
+        <v>115099</v>
+      </c>
+      <c r="D32" s="11">
+        <v>1.885</v>
+      </c>
+      <c r="E32" s="9">
+        <v>119</v>
+      </c>
+      <c r="F32" s="7">
+        <v>22.73</v>
+      </c>
+      <c r="G32" s="7">
+        <v>44.64</v>
+      </c>
+      <c r="H32" s="7">
+        <v>45.12</v>
+      </c>
+      <c r="I32" s="7">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="J32" s="6">
+        <v>-0.3</v>
+      </c>
+      <c r="K32" s="9">
+        <v>22.5</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="2">
+        <v>207268</v>
+      </c>
+      <c r="D33" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E33" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F33" s="7">
+        <v>22.97</v>
+      </c>
+      <c r="G33" s="7">
+        <v>42.03</v>
+      </c>
+      <c r="H33" s="7">
+        <v>43.1</v>
+      </c>
+      <c r="I33" s="7">
+        <v>2.68</v>
+      </c>
+      <c r="J33" s="6">
+        <v>-0.2</v>
+      </c>
+      <c r="K33" s="9">
+        <v>24.5</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2">
+        <v>209451</v>
+      </c>
+      <c r="D34" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E34" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F34" s="7">
+        <v>22.96</v>
+      </c>
+      <c r="G34" s="7">
+        <v>42.51</v>
+      </c>
+      <c r="H34" s="7">
+        <v>43.83</v>
+      </c>
+      <c r="I34" s="7">
+        <v>2.56</v>
+      </c>
+      <c r="J34" s="6">
+        <v>-0.2</v>
+      </c>
+      <c r="K34" s="9">
+        <v>24</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="2">
+        <v>46462</v>
+      </c>
+      <c r="D35" s="11">
+        <v>2.04</v>
+      </c>
+      <c r="E35" s="9">
+        <v>119.3</v>
+      </c>
+      <c r="F35" s="7">
+        <v>22.56</v>
+      </c>
+      <c r="G35" s="7">
+        <v>44.76</v>
+      </c>
+      <c r="H35" s="7">
+        <v>45.3</v>
+      </c>
+      <c r="I35" s="7">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="J35" s="6">
+        <v>-0.37</v>
+      </c>
+      <c r="K35" s="9">
+        <v>23.5</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="B4:D1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix(barrett_calculator.py): update backup file naming convention for results file
</commit_message>
<xml_diff>
--- a/APACdata.xlsx
+++ b/APACdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yokam\PycharmProjects\BarrettAutomate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159B980A-4776-443E-BA09-438388DC6AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397D76AE-D8F3-48B7-ADBB-3AD98F61CEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="465" windowWidth="22650" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="720" windowWidth="26190" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="36" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
   <si>
     <t>Optic</t>
   </si>
@@ -87,27 +87,6 @@
     <t>attack03</t>
   </si>
   <si>
-    <t>attack05</t>
-  </si>
-  <si>
-    <t>attack07</t>
-  </si>
-  <si>
-    <t>attack09</t>
-  </si>
-  <si>
-    <t>attack15</t>
-  </si>
-  <si>
-    <t>attack23</t>
-  </si>
-  <si>
-    <t>attack26</t>
-  </si>
-  <si>
-    <t>attack30</t>
-  </si>
-  <si>
     <t>KFLADA</t>
   </si>
   <si>
@@ -124,6 +103,15 @@
   </si>
   <si>
     <t>KFLFDF</t>
+  </si>
+  <si>
+    <t>attack01</t>
+  </si>
+  <si>
+    <t>KALADA</t>
+  </si>
+  <si>
+    <t>KALADF</t>
   </si>
 </sst>
 </file>
@@ -550,9 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -609,13 +595,13 @@
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1">
-        <v>133873</v>
+        <v>105737</v>
       </c>
       <c r="D2" s="11">
         <v>1.88</v>
@@ -624,22 +610,22 @@
         <v>118.99</v>
       </c>
       <c r="F2" s="7">
-        <v>23.17</v>
+        <v>23.33</v>
       </c>
       <c r="G2" s="7">
-        <v>46.5</v>
+        <v>44.75</v>
       </c>
       <c r="H2" s="7">
-        <v>48.25</v>
+        <v>44.25</v>
       </c>
       <c r="I2" s="7">
-        <v>1.81</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="J2" s="7">
-        <v>-0.53</v>
+        <v>-0.03</v>
       </c>
       <c r="K2" s="9">
-        <v>22</v>
+        <v>21.5</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>1</v>
@@ -647,13 +633,13 @@
     </row>
     <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="1">
-        <v>132594</v>
+        <v>133873</v>
       </c>
       <c r="D3" s="11">
         <v>1.88</v>
@@ -662,22 +648,22 @@
         <v>118.99</v>
       </c>
       <c r="F3" s="7">
-        <v>21.64</v>
+        <v>23.17</v>
       </c>
       <c r="G3" s="7">
-        <v>44.25</v>
+        <v>43.75</v>
       </c>
       <c r="H3" s="7">
-        <v>44</v>
+        <v>44.5</v>
       </c>
       <c r="I3" s="7">
-        <v>2.73</v>
+        <v>1.81</v>
       </c>
       <c r="J3" s="7">
-        <v>-0.96</v>
+        <v>-0.53</v>
       </c>
       <c r="K3" s="9">
-        <v>24.5</v>
+        <v>22</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -685,37 +671,37 @@
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="2">
-        <v>110627</v>
+        <v>132594</v>
       </c>
       <c r="D4" s="11">
-        <v>2.09</v>
+        <v>1.88</v>
       </c>
       <c r="E4" s="9">
-        <v>119.39</v>
+        <v>118.99</v>
       </c>
       <c r="F4" s="7">
-        <v>22.05</v>
+        <v>21.64</v>
       </c>
       <c r="G4" s="7">
-        <v>44.29</v>
+        <v>46.75</v>
       </c>
       <c r="H4" s="7">
-        <v>48.49</v>
+        <v>48.5</v>
       </c>
       <c r="I4" s="7">
-        <v>2.3199999999999998</v>
+        <v>2.73</v>
       </c>
       <c r="J4" s="6">
-        <v>-0.88</v>
+        <v>-0.96</v>
       </c>
       <c r="K4" s="9">
-        <v>26.5</v>
+        <v>24.5</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>1</v>
@@ -723,13 +709,13 @@
     </row>
     <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2">
-        <v>184985</v>
+        <v>105737</v>
       </c>
       <c r="D5" s="11">
         <v>1.88</v>
@@ -738,22 +724,22 @@
         <v>118.99</v>
       </c>
       <c r="F5" s="7">
-        <v>22.11</v>
+        <v>23.04</v>
       </c>
       <c r="G5" s="7">
-        <v>44.53</v>
+        <v>44.75</v>
       </c>
       <c r="H5" s="7">
-        <v>46.11</v>
+        <v>44.25</v>
       </c>
       <c r="I5" s="7">
         <v>2.1800000000000002</v>
       </c>
       <c r="J5" s="6">
-        <v>-0.09</v>
+        <v>-0.03</v>
       </c>
       <c r="K5" s="9">
-        <v>26</v>
+        <v>21.5</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>1</v>
@@ -764,7 +750,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2">
         <v>133873</v>
@@ -776,7 +762,7 @@
         <v>118.99</v>
       </c>
       <c r="F6" s="7">
-        <v>21.68</v>
+        <v>22.79</v>
       </c>
       <c r="G6" s="7">
         <v>43.75</v>
@@ -802,7 +788,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2">
         <v>132594</v>
@@ -814,7 +800,7 @@
         <v>118.99</v>
       </c>
       <c r="F7" s="7">
-        <v>22.79</v>
+        <v>21.68</v>
       </c>
       <c r="G7" s="7">
         <v>46.75</v>
@@ -837,13 +823,13 @@
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
-        <v>35135</v>
+        <v>105737</v>
       </c>
       <c r="D8" s="11">
         <v>1.88</v>
@@ -852,22 +838,22 @@
         <v>118.99</v>
       </c>
       <c r="F8" s="7">
-        <v>21.78</v>
+        <v>23.33</v>
       </c>
       <c r="G8" s="7">
-        <v>42.56</v>
+        <v>45.25</v>
       </c>
       <c r="H8" s="7">
-        <v>43.44</v>
+        <v>43.25</v>
       </c>
       <c r="I8" s="7">
-        <v>3.16</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="J8" s="6">
-        <v>-0.3</v>
+        <v>-0.03</v>
       </c>
       <c r="K8" s="9">
-        <v>25.5</v>
+        <v>21.5</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>1</v>
@@ -875,13 +861,13 @@
     </row>
     <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" s="2">
-        <v>143993</v>
+        <v>133873</v>
       </c>
       <c r="D9" s="11">
         <v>1.88</v>
@@ -890,22 +876,22 @@
         <v>118.99</v>
       </c>
       <c r="F9" s="7">
-        <v>24.09</v>
+        <v>23.17</v>
       </c>
       <c r="G9" s="7">
-        <v>43.05</v>
+        <v>44.25</v>
       </c>
       <c r="H9" s="7">
-        <v>44.41</v>
+        <v>44</v>
       </c>
       <c r="I9" s="7">
-        <v>2.27</v>
+        <v>1.81</v>
       </c>
       <c r="J9" s="6">
-        <v>-0.6</v>
+        <v>-0.53</v>
       </c>
       <c r="K9" s="9">
-        <v>22.5</v>
+        <v>22</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>1</v>
@@ -913,13 +899,13 @@
     </row>
     <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2">
-        <v>51973</v>
+        <v>132594</v>
       </c>
       <c r="D10" s="11">
         <v>1.88</v>
@@ -928,22 +914,22 @@
         <v>118.99</v>
       </c>
       <c r="F10" s="7">
-        <v>21.25</v>
+        <v>21.64</v>
       </c>
       <c r="G10" s="7">
-        <v>44.76</v>
+        <v>46.5</v>
       </c>
       <c r="H10" s="7">
-        <v>47.47</v>
+        <v>48.25</v>
       </c>
       <c r="I10" s="7">
-        <v>2.0499999999999998</v>
+        <v>2.73</v>
       </c>
       <c r="J10" s="6">
-        <v>-1.29</v>
+        <v>-0.96</v>
       </c>
       <c r="K10" s="9">
-        <v>26</v>
+        <v>24.5</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>1</v>
@@ -951,13 +937,13 @@
     </row>
     <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>125842</v>
+        <v>105737</v>
       </c>
       <c r="D11" s="11">
         <v>1.88</v>
@@ -966,22 +952,22 @@
         <v>118.99</v>
       </c>
       <c r="F11" s="7">
-        <v>22.3</v>
+        <v>23.33</v>
       </c>
       <c r="G11" s="7">
-        <v>43.5</v>
+        <v>44.75</v>
       </c>
       <c r="H11" s="7">
-        <v>46</v>
+        <v>44.25</v>
       </c>
       <c r="I11" s="7">
-        <v>2.75</v>
+        <v>2.33</v>
       </c>
       <c r="J11" s="6">
-        <v>-0.1</v>
+        <v>-0.03</v>
       </c>
       <c r="K11" s="9">
-        <v>28</v>
+        <v>21.5</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>1</v>
@@ -989,37 +975,37 @@
     </row>
     <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="2">
-        <v>198772</v>
+        <v>133873</v>
       </c>
       <c r="D12" s="11">
-        <v>2.09</v>
+        <v>1.88</v>
       </c>
       <c r="E12" s="9">
-        <v>119.39</v>
+        <v>118.99</v>
       </c>
       <c r="F12" s="7">
-        <v>21.49</v>
+        <v>23.17</v>
       </c>
       <c r="G12" s="7">
-        <v>42.61</v>
+        <v>43.75</v>
       </c>
       <c r="H12" s="7">
-        <v>43.32</v>
+        <v>44.5</v>
       </c>
       <c r="I12" s="7">
-        <v>2.4900000000000002</v>
+        <v>2.44</v>
       </c>
       <c r="J12" s="6">
-        <v>-0.22</v>
+        <v>-0.53</v>
       </c>
       <c r="K12" s="9">
-        <v>28.5</v>
+        <v>22</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>1</v>
@@ -1027,13 +1013,13 @@
     </row>
     <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2">
-        <v>35135</v>
+        <v>132594</v>
       </c>
       <c r="D13" s="11">
         <v>1.88</v>
@@ -1042,22 +1028,22 @@
         <v>118.99</v>
       </c>
       <c r="F13" s="7">
-        <v>21.78</v>
+        <v>21.64</v>
       </c>
       <c r="G13" s="7">
-        <v>43.1</v>
+        <v>46.75</v>
       </c>
       <c r="H13" s="7">
-        <v>45</v>
+        <v>48.5</v>
       </c>
       <c r="I13" s="7">
-        <v>3.16</v>
+        <v>3.05</v>
       </c>
       <c r="J13" s="6">
-        <v>-0.3</v>
+        <v>-0.96</v>
       </c>
       <c r="K13" s="9">
-        <v>25.5</v>
+        <v>24.5</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>1</v>
@@ -1065,13 +1051,13 @@
     </row>
     <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2">
-        <v>143993</v>
+        <v>105737</v>
       </c>
       <c r="D14" s="11">
         <v>1.88</v>
@@ -1080,22 +1066,22 @@
         <v>118.99</v>
       </c>
       <c r="F14" s="7">
-        <v>24.09</v>
+        <v>23.04</v>
       </c>
       <c r="G14" s="7">
-        <v>43.44</v>
+        <v>45.25</v>
       </c>
       <c r="H14" s="7">
-        <v>43.83</v>
+        <v>43.25</v>
       </c>
       <c r="I14" s="7">
-        <v>2.27</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="J14" s="6">
-        <v>-0.6</v>
+        <v>-0.03</v>
       </c>
       <c r="K14" s="9">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>1</v>
@@ -1103,13 +1089,13 @@
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2">
-        <v>125842</v>
+        <v>133873</v>
       </c>
       <c r="D15" s="11">
         <v>1.88</v>
@@ -1118,22 +1104,22 @@
         <v>118.99</v>
       </c>
       <c r="F15" s="7">
-        <v>22.3</v>
+        <v>22.79</v>
       </c>
       <c r="G15" s="7">
-        <v>45.18</v>
+        <v>44.25</v>
       </c>
       <c r="H15" s="7">
-        <v>45.42</v>
+        <v>44</v>
       </c>
       <c r="I15" s="7">
-        <v>2.75</v>
+        <v>1.81</v>
       </c>
       <c r="J15" s="6">
-        <v>-0.1</v>
+        <v>-0.53</v>
       </c>
       <c r="K15" s="9">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>1</v>
@@ -1141,37 +1127,37 @@
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2">
-        <v>198772</v>
+        <v>132594</v>
       </c>
       <c r="D16" s="11">
-        <v>2.09</v>
+        <v>1.88</v>
       </c>
       <c r="E16" s="9">
-        <v>119.39</v>
+        <v>118.99</v>
       </c>
       <c r="F16" s="7">
-        <v>21.49</v>
+        <v>21.68</v>
       </c>
       <c r="G16" s="7">
-        <v>42.08</v>
+        <v>46.5</v>
       </c>
       <c r="H16" s="7">
-        <v>42.94</v>
+        <v>48.25</v>
       </c>
       <c r="I16" s="7">
-        <v>2.4900000000000002</v>
+        <v>2.73</v>
       </c>
       <c r="J16" s="6">
-        <v>-0.22</v>
+        <v>-0.96</v>
       </c>
       <c r="K16" s="9">
-        <v>28.5</v>
+        <v>24.5</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>1</v>
@@ -1179,13 +1165,13 @@
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2">
-        <v>133873</v>
+        <v>105737</v>
       </c>
       <c r="D17" s="11">
         <v>1.88</v>
@@ -1194,22 +1180,22 @@
         <v>118.99</v>
       </c>
       <c r="F17" s="7">
-        <v>23.17</v>
+        <v>23.04</v>
       </c>
       <c r="G17" s="7">
-        <v>46.5</v>
+        <v>44.75</v>
       </c>
       <c r="H17" s="7">
-        <v>48.25</v>
+        <v>44.25</v>
       </c>
       <c r="I17" s="7">
-        <v>3.05</v>
+        <v>2.33</v>
       </c>
       <c r="J17" s="6">
-        <v>-0.53</v>
+        <v>-0.03</v>
       </c>
       <c r="K17" s="9">
-        <v>22</v>
+        <v>21.5</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>1</v>
@@ -1217,13 +1203,13 @@
     </row>
     <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2">
-        <v>132594</v>
+        <v>133873</v>
       </c>
       <c r="D18" s="11">
         <v>1.88</v>
@@ -1232,22 +1218,22 @@
         <v>118.99</v>
       </c>
       <c r="F18" s="7">
-        <v>21.64</v>
+        <v>22.79</v>
       </c>
       <c r="G18" s="7">
-        <v>44.25</v>
+        <v>43.75</v>
       </c>
       <c r="H18" s="7">
-        <v>44</v>
+        <v>44.5</v>
       </c>
       <c r="I18" s="7">
         <v>2.44</v>
       </c>
       <c r="J18" s="6">
-        <v>-0.96</v>
+        <v>-0.53</v>
       </c>
       <c r="K18" s="9">
-        <v>24.5</v>
+        <v>22</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>1</v>
@@ -1255,37 +1241,37 @@
     </row>
     <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2">
-        <v>110627</v>
+        <v>132594</v>
       </c>
       <c r="D19" s="11">
-        <v>2.09</v>
+        <v>1.88</v>
       </c>
       <c r="E19" s="9">
-        <v>119.39</v>
+        <v>118.99</v>
       </c>
       <c r="F19" s="7">
-        <v>22.05</v>
+        <v>21.68</v>
       </c>
       <c r="G19" s="7">
-        <v>44.29</v>
+        <v>46.75</v>
       </c>
       <c r="H19" s="7">
-        <v>48.49</v>
+        <v>48.5</v>
       </c>
       <c r="I19" s="7">
-        <v>2.35</v>
+        <v>3.05</v>
       </c>
       <c r="J19" s="6">
-        <v>-0.88</v>
+        <v>-0.96</v>
       </c>
       <c r="K19" s="9">
-        <v>26.5</v>
+        <v>24.5</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>1</v>
@@ -1293,13 +1279,13 @@
     </row>
     <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C20" s="2">
-        <v>184985</v>
+        <v>105737</v>
       </c>
       <c r="D20" s="11">
         <v>1.88</v>
@@ -1308,22 +1294,22 @@
         <v>118.99</v>
       </c>
       <c r="F20" s="7">
-        <v>22.11</v>
+        <v>23.33</v>
       </c>
       <c r="G20" s="7">
-        <v>44.53</v>
+        <v>45.25</v>
       </c>
       <c r="H20" s="7">
-        <v>46.11</v>
+        <v>43.25</v>
       </c>
       <c r="I20" s="7">
-        <v>2.36</v>
+        <v>2.33</v>
       </c>
       <c r="J20" s="6">
-        <v>-0.09</v>
+        <v>-0.03</v>
       </c>
       <c r="K20" s="9">
-        <v>26</v>
+        <v>21.5</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>1</v>
@@ -1334,7 +1320,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2">
         <v>133873</v>
@@ -1346,16 +1332,16 @@
         <v>118.99</v>
       </c>
       <c r="F21" s="7">
-        <v>21.68</v>
+        <v>23.17</v>
       </c>
       <c r="G21" s="7">
-        <v>43.75</v>
+        <v>44.25</v>
       </c>
       <c r="H21" s="7">
-        <v>44.5</v>
+        <v>44</v>
       </c>
       <c r="I21" s="7">
-        <v>3.05</v>
+        <v>2.44</v>
       </c>
       <c r="J21" s="6">
         <v>-0.53</v>
@@ -1372,7 +1358,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2">
         <v>132594</v>
@@ -1384,16 +1370,16 @@
         <v>118.99</v>
       </c>
       <c r="F22" s="7">
-        <v>22.79</v>
+        <v>21.64</v>
       </c>
       <c r="G22" s="7">
-        <v>46.75</v>
+        <v>46.5</v>
       </c>
       <c r="H22" s="7">
-        <v>48.5</v>
+        <v>48.25</v>
       </c>
       <c r="I22" s="7">
-        <v>2.44</v>
+        <v>3.05</v>
       </c>
       <c r="J22" s="6">
         <v>-0.96</v>
@@ -1407,13 +1393,13 @@
     </row>
     <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2">
-        <v>35135</v>
+        <v>105737</v>
       </c>
       <c r="D23" s="11">
         <v>1.88</v>
@@ -1422,22 +1408,22 @@
         <v>118.99</v>
       </c>
       <c r="F23" s="7">
-        <v>21.78</v>
+        <v>23.04</v>
       </c>
       <c r="G23" s="7">
-        <v>42.56</v>
+        <v>45.25</v>
       </c>
       <c r="H23" s="7">
-        <v>43.44</v>
+        <v>43.25</v>
       </c>
       <c r="I23" s="7">
-        <v>2.75</v>
+        <v>2.33</v>
       </c>
       <c r="J23" s="6">
-        <v>-0.3</v>
+        <v>-0.03</v>
       </c>
       <c r="K23" s="9">
-        <v>25.5</v>
+        <v>21.5</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>1</v>
@@ -1445,13 +1431,13 @@
     </row>
     <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2">
-        <v>143993</v>
+        <v>133873</v>
       </c>
       <c r="D24" s="11">
         <v>1.88</v>
@@ -1460,22 +1446,22 @@
         <v>118.99</v>
       </c>
       <c r="F24" s="7">
-        <v>24.09</v>
+        <v>22.79</v>
       </c>
       <c r="G24" s="7">
-        <v>43.05</v>
+        <v>44.25</v>
       </c>
       <c r="H24" s="7">
-        <v>44.41</v>
+        <v>44</v>
       </c>
       <c r="I24" s="7">
-        <v>2.29</v>
+        <v>2.44</v>
       </c>
       <c r="J24" s="6">
-        <v>-0.6</v>
+        <v>-0.53</v>
       </c>
       <c r="K24" s="9">
-        <v>22.5</v>
+        <v>22</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>1</v>
@@ -1483,13 +1469,13 @@
     </row>
     <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2">
-        <v>51973</v>
+        <v>132594</v>
       </c>
       <c r="D25" s="11">
         <v>1.88</v>
@@ -1498,254 +1484,50 @@
         <v>118.99</v>
       </c>
       <c r="F25" s="7">
-        <v>21.25</v>
+        <v>21.68</v>
       </c>
       <c r="G25" s="7">
-        <v>44.76</v>
+        <v>46.5</v>
       </c>
       <c r="H25" s="7">
-        <v>47.47</v>
+        <v>48.25</v>
       </c>
       <c r="I25" s="7">
-        <v>2.29</v>
+        <v>3.05</v>
       </c>
       <c r="J25" s="6">
-        <v>-1.29</v>
+        <v>-0.96</v>
       </c>
       <c r="K25" s="9">
-        <v>26</v>
+        <v>24.5</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="2">
-        <v>125842</v>
-      </c>
-      <c r="D26" s="11">
-        <v>1.88</v>
-      </c>
-      <c r="E26" s="9">
-        <v>118.99</v>
-      </c>
-      <c r="F26" s="7">
-        <v>22.3</v>
-      </c>
-      <c r="G26" s="7">
-        <v>43.5</v>
-      </c>
-      <c r="H26" s="7">
-        <v>46</v>
-      </c>
-      <c r="I26" s="7">
-        <v>2.52</v>
-      </c>
-      <c r="J26" s="6">
-        <v>-0.1</v>
-      </c>
-      <c r="K26" s="9">
-        <v>28</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="11"/>
     </row>
     <row r="27" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="2">
-        <v>198772</v>
-      </c>
-      <c r="D27" s="11">
-        <v>2.09</v>
-      </c>
-      <c r="E27" s="9">
-        <v>119.39</v>
-      </c>
-      <c r="F27" s="7">
-        <v>21.49</v>
-      </c>
-      <c r="G27" s="7">
-        <v>42.61</v>
-      </c>
-      <c r="H27" s="7">
-        <v>43.32</v>
-      </c>
-      <c r="I27" s="7">
-        <v>2.19</v>
-      </c>
-      <c r="J27" s="6">
-        <v>-0.22</v>
-      </c>
-      <c r="K27" s="9">
-        <v>28.5</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="2">
-        <v>133873</v>
-      </c>
-      <c r="D28" s="11">
-        <v>1.88</v>
-      </c>
-      <c r="E28" s="9">
-        <v>118.99</v>
-      </c>
-      <c r="F28" s="7">
-        <v>21.68</v>
-      </c>
-      <c r="G28" s="7">
-        <v>46.5</v>
-      </c>
-      <c r="H28" s="7">
-        <v>48.25</v>
-      </c>
-      <c r="I28" s="7">
-        <v>3.05</v>
-      </c>
-      <c r="J28" s="6">
-        <v>-0.53</v>
-      </c>
-      <c r="K28" s="9">
-        <v>22</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="2">
-        <v>143993</v>
-      </c>
-      <c r="D29" s="11">
-        <v>1.88</v>
-      </c>
-      <c r="E29" s="9">
-        <v>118.99</v>
-      </c>
-      <c r="F29" s="7">
-        <v>24.09</v>
-      </c>
-      <c r="G29" s="7">
-        <v>43.44</v>
-      </c>
-      <c r="H29" s="7">
-        <v>43.83</v>
-      </c>
-      <c r="I29" s="7">
-        <v>2.29</v>
-      </c>
-      <c r="J29" s="6">
-        <v>-0.6</v>
-      </c>
-      <c r="K29" s="9">
-        <v>22.5</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="2">
-        <v>125842</v>
-      </c>
-      <c r="D30" s="11">
-        <v>1.88</v>
-      </c>
-      <c r="E30" s="9">
-        <v>118.99</v>
-      </c>
-      <c r="F30" s="7">
-        <v>22.3</v>
-      </c>
-      <c r="G30" s="7">
-        <v>45.18</v>
-      </c>
-      <c r="H30" s="7">
-        <v>45.42</v>
-      </c>
-      <c r="I30" s="7">
-        <v>2.52</v>
-      </c>
-      <c r="J30" s="6">
-        <v>-0.1</v>
-      </c>
-      <c r="K30" s="9">
-        <v>28</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="2">
-        <v>198772</v>
-      </c>
-      <c r="D31" s="11">
-        <v>2.09</v>
-      </c>
-      <c r="E31" s="9">
-        <v>119.39</v>
-      </c>
-      <c r="F31" s="7">
-        <v>21.49</v>
-      </c>
-      <c r="G31" s="7">
-        <v>42.08</v>
-      </c>
-      <c r="H31" s="7">
-        <v>42.94</v>
-      </c>
-      <c r="I31" s="7">
-        <v>2.19</v>
-      </c>
-      <c r="J31" s="6">
-        <v>-0.22</v>
-      </c>
-      <c r="K31" s="9">
-        <v>28.5</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="1"/>

</xml_diff>